<commit_message>
will match star_ID from Ralf for HIP and GJ numbers
</commit_message>
<xml_diff>
--- a/results/merged_RJ.xlsx
+++ b/results/merged_RJ.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BU258"/>
+  <dimension ref="A1:BV258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -797,6 +797,11 @@
       <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>V_mag_group</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>HZ Detection Limit Simplified [Earth Mass]</t>
         </is>
       </c>
     </row>
@@ -976,6 +981,7 @@
       <c r="BS2" t="inlineStr"/>
       <c r="BT2" t="inlineStr"/>
       <c r="BU2" t="inlineStr"/>
+      <c r="BV2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1226,6 +1232,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV3" t="n">
+        <v>1.621444358408722</v>
       </c>
     </row>
     <row r="4">
@@ -1404,6 +1413,7 @@
       <c r="BS4" t="inlineStr"/>
       <c r="BT4" t="inlineStr"/>
       <c r="BU4" t="inlineStr"/>
+      <c r="BV4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1581,6 +1591,7 @@
       <c r="BS5" t="inlineStr"/>
       <c r="BT5" t="inlineStr"/>
       <c r="BU5" t="inlineStr"/>
+      <c r="BV5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1762,6 +1773,7 @@
       <c r="BS6" t="inlineStr"/>
       <c r="BT6" t="inlineStr"/>
       <c r="BU6" t="inlineStr"/>
+      <c r="BV6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2012,6 +2024,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV7" t="n">
+        <v>1.484919117162514</v>
       </c>
     </row>
     <row r="8">
@@ -2190,6 +2205,7 @@
       <c r="BS8" t="inlineStr"/>
       <c r="BT8" t="inlineStr"/>
       <c r="BU8" t="inlineStr"/>
+      <c r="BV8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2437,6 +2453,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV9" t="n">
+        <v>0.7628367688271928</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2688,6 +2707,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV10" t="n">
+        <v>1.184254862123319</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2931,6 +2953,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV11" t="n">
+        <v>1.579134434740717</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3177,6 +3202,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV12" t="n">
+        <v>0.5858296028846899</v>
       </c>
     </row>
     <row r="13">
@@ -3355,6 +3383,7 @@
       <c r="BS13" t="inlineStr"/>
       <c r="BT13" t="inlineStr"/>
       <c r="BU13" t="inlineStr"/>
+      <c r="BV13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3602,6 +3631,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV14" t="n">
+        <v>1.36954269712146</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3849,6 +3881,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV15" t="n">
+        <v>4.998399480393742</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -4096,6 +4131,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV16" t="n">
+        <v>2.249839030061863</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -4343,6 +4381,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV17" t="n">
+        <v>1.103876207198841</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -4593,6 +4634,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV18" t="n">
+        <v>1.788390570247163</v>
       </c>
     </row>
     <row r="19">
@@ -4771,6 +4815,7 @@
       <c r="BS19" t="inlineStr"/>
       <c r="BT19" t="inlineStr"/>
       <c r="BU19" t="inlineStr"/>
+      <c r="BV19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -4948,6 +4993,7 @@
       <c r="BS20" t="inlineStr"/>
       <c r="BT20" t="inlineStr"/>
       <c r="BU20" t="inlineStr"/>
+      <c r="BV20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -5195,6 +5241,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV21" t="n">
+        <v>1.438971115600265</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -5438,6 +5487,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV22" t="n">
+        <v>0.6408543957456876</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -5685,6 +5737,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV23" t="n">
+        <v>1.903430525974275</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -5932,6 +5987,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV24" t="n">
+        <v>0.5618021102691635</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -6183,6 +6241,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV25" t="n">
+        <v>0.303361852725467</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -6434,6 +6495,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV26" t="n">
+        <v>0.8448969923111</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -6685,6 +6749,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV27" t="n">
+        <v>0.954190334896956</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -6931,6 +6998,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV28" t="n">
+        <v>2.157678897671709</v>
       </c>
     </row>
     <row r="29">
@@ -7109,6 +7179,7 @@
       <c r="BS29" t="inlineStr"/>
       <c r="BT29" t="inlineStr"/>
       <c r="BU29" t="inlineStr"/>
+      <c r="BV29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -7355,6 +7426,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV30" t="n">
+        <v>0.5987243514626134</v>
       </c>
     </row>
     <row r="31">
@@ -7533,6 +7607,7 @@
       <c r="BS31" t="inlineStr"/>
       <c r="BT31" t="inlineStr"/>
       <c r="BU31" t="inlineStr"/>
+      <c r="BV31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -7779,6 +7854,9 @@
         <is>
           <t>Brightest</t>
         </is>
+      </c>
+      <c r="BV32" t="n">
+        <v>1.589883367965815</v>
       </c>
     </row>
     <row r="33">
@@ -7957,6 +8035,7 @@
       <c r="BS33" t="inlineStr"/>
       <c r="BT33" t="inlineStr"/>
       <c r="BU33" t="inlineStr"/>
+      <c r="BV33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -8207,6 +8286,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV34" t="n">
+        <v>0.7319332528441378</v>
       </c>
     </row>
     <row r="35">
@@ -8385,6 +8467,7 @@
       <c r="BS35" t="inlineStr"/>
       <c r="BT35" t="inlineStr"/>
       <c r="BU35" t="inlineStr"/>
+      <c r="BV35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -8562,6 +8645,7 @@
       <c r="BS36" t="inlineStr"/>
       <c r="BT36" t="inlineStr"/>
       <c r="BU36" t="inlineStr"/>
+      <c r="BV36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -8739,6 +8823,7 @@
       <c r="BS37" t="inlineStr"/>
       <c r="BT37" t="inlineStr"/>
       <c r="BU37" t="inlineStr"/>
+      <c r="BV37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -8990,6 +9075,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV38" t="n">
+        <v>1.942149178380478</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -9241,6 +9329,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV39" t="n">
+        <v>0.9615074465357535</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -9492,6 +9583,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV40" t="n">
+        <v>0.9471067378845955</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -9735,6 +9829,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV41" t="n">
+        <v>0.7151688901656719</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -9985,6 +10082,9 @@
         <is>
           <t>Brightest</t>
         </is>
+      </c>
+      <c r="BV42" t="n">
+        <v>0.4365665462772206</v>
       </c>
     </row>
     <row r="43">
@@ -10163,6 +10263,7 @@
       <c r="BS43" t="inlineStr"/>
       <c r="BT43" t="inlineStr"/>
       <c r="BU43" t="inlineStr"/>
+      <c r="BV43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -10414,6 +10515,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV44" t="n">
+        <v>1.441900852959071</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -10661,6 +10765,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV45" t="n">
+        <v>1.339159232533579</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -10912,6 +11019,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV46" t="n">
+        <v>1.470889643181826</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -11163,6 +11273,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV47" t="n">
+        <v>0.2467370832682639</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -11413,6 +11526,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV48" t="n">
+        <v>1.225956103360744</v>
       </c>
     </row>
     <row r="49">
@@ -11591,6 +11707,7 @@
       <c r="BS49" t="inlineStr"/>
       <c r="BT49" t="inlineStr"/>
       <c r="BU49" t="inlineStr"/>
+      <c r="BV49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -11838,6 +11955,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV50" t="n">
+        <v>1.105551856874697</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -12084,6 +12204,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV51" t="n">
+        <v>1.202259761373707</v>
       </c>
     </row>
     <row r="52">
@@ -12262,6 +12385,7 @@
       <c r="BS52" t="inlineStr"/>
       <c r="BT52" t="inlineStr"/>
       <c r="BU52" t="inlineStr"/>
+      <c r="BV52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -12508,6 +12632,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV53" t="n">
+        <v>1.858372141892437</v>
       </c>
     </row>
     <row r="54">
@@ -12690,6 +12817,7 @@
       <c r="BS54" t="inlineStr"/>
       <c r="BT54" t="inlineStr"/>
       <c r="BU54" t="inlineStr"/>
+      <c r="BV54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -12937,6 +13065,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV55" t="n">
+        <v>7.305162650746633</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -13188,6 +13319,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV56" t="n">
+        <v>0.4046871584426158</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -13435,6 +13569,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV57" t="n">
+        <v>1.19098817920673</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -13682,6 +13819,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV58" t="n">
+        <v>1.190675342837873</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -13932,6 +14072,9 @@
         <is>
           <t>Brightest</t>
         </is>
+      </c>
+      <c r="BV59" t="n">
+        <v>1.005987451437576</v>
       </c>
     </row>
     <row r="60">
@@ -14110,6 +14253,7 @@
       <c r="BS60" t="inlineStr"/>
       <c r="BT60" t="inlineStr"/>
       <c r="BU60" t="inlineStr"/>
+      <c r="BV60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -14361,6 +14505,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV61" t="n">
+        <v>1.324072949522606</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -14608,6 +14755,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV62" t="n">
+        <v>1.572277001130793</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -14859,6 +15009,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV63" t="n">
+        <v>0.6777585808931341</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -15105,6 +15258,9 @@
         <is>
           <t>Brightest</t>
         </is>
+      </c>
+      <c r="BV64" t="n">
+        <v>1.943243680416653</v>
       </c>
     </row>
     <row r="65">
@@ -15283,6 +15439,7 @@
       <c r="BS65" t="inlineStr"/>
       <c r="BT65" t="inlineStr"/>
       <c r="BU65" t="inlineStr"/>
+      <c r="BV65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -15530,6 +15687,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV66" t="n">
+        <v>1.346038523514871</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -15777,6 +15937,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV67" t="n">
+        <v>3.131437408085968</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -16024,6 +16187,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV68" t="n">
+        <v>1.933288290662833</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -16275,6 +16441,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV69" t="n">
+        <v>1.438505336044193</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -16522,6 +16691,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV70" t="n">
+        <v>1.382470712463236</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -16772,6 +16944,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV71" t="n">
+        <v>1.150702425643469</v>
       </c>
     </row>
     <row r="72">
@@ -16950,6 +17125,7 @@
       <c r="BS72" t="inlineStr"/>
       <c r="BT72" t="inlineStr"/>
       <c r="BU72" t="inlineStr"/>
+      <c r="BV72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -17197,6 +17373,9 @@
           <t>Dimmer</t>
         </is>
       </c>
+      <c r="BV73" t="n">
+        <v>2.149681965874837</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -17444,6 +17623,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV74" t="n">
+        <v>1.374984737118</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -17687,6 +17869,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV75" t="n">
+        <v>0.7100546668150038</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -17930,6 +18115,9 @@
         <v>8.905034452470854</v>
       </c>
       <c r="BU76" t="inlineStr"/>
+      <c r="BV76" t="n">
+        <v>3.556120824975452</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -18181,6 +18369,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV77" t="n">
+        <v>1.200323763972236</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -18432,6 +18623,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV78" t="n">
+        <v>1.054040447621109</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -18683,6 +18877,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV79" t="n">
+        <v>1.096137089666106</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -18930,6 +19127,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV80" t="n">
+        <v>0.7252878618234446</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -19181,6 +19381,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV81" t="n">
+        <v>1.453543344712819</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -19427,6 +19630,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV82" t="n">
+        <v>1.269488462238789</v>
       </c>
     </row>
     <row r="83">
@@ -19605,6 +19811,7 @@
       <c r="BS83" t="inlineStr"/>
       <c r="BT83" t="inlineStr"/>
       <c r="BU83" t="inlineStr"/>
+      <c r="BV83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -19782,6 +19989,7 @@
       <c r="BS84" t="inlineStr"/>
       <c r="BT84" t="inlineStr"/>
       <c r="BU84" t="inlineStr"/>
+      <c r="BV84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -20033,6 +20241,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV85" t="n">
+        <v>0.9284413491685983</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -20279,6 +20490,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV86" t="n">
+        <v>10.8912648986421</v>
       </c>
     </row>
     <row r="87">
@@ -20457,6 +20671,7 @@
       <c r="BS87" t="inlineStr"/>
       <c r="BT87" t="inlineStr"/>
       <c r="BU87" t="inlineStr"/>
+      <c r="BV87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -20708,6 +20923,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV88" t="n">
+        <v>1.2567515127527</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -20955,6 +21173,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV89" t="n">
+        <v>1.035484286571943</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -21205,6 +21426,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV90" t="n">
+        <v>1.699558719045058</v>
       </c>
     </row>
     <row r="91">
@@ -21383,6 +21607,7 @@
       <c r="BS91" t="inlineStr"/>
       <c r="BT91" t="inlineStr"/>
       <c r="BU91" t="inlineStr"/>
+      <c r="BV91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -21630,6 +21855,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV92" t="n">
+        <v>1.913164835210601</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -21877,6 +22105,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV93" t="n">
+        <v>1.055130165447589</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -22120,6 +22351,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV94" t="n">
+        <v>1.486154076822704</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -22362,6 +22596,9 @@
         <is>
           <t>Brightest</t>
         </is>
+      </c>
+      <c r="BV95" t="n">
+        <v>16.87830163415827</v>
       </c>
     </row>
     <row r="96">
@@ -22544,6 +22781,7 @@
       <c r="BS96" t="inlineStr"/>
       <c r="BT96" t="inlineStr"/>
       <c r="BU96" t="inlineStr"/>
+      <c r="BV96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -22721,6 +22959,7 @@
       <c r="BS97" t="inlineStr"/>
       <c r="BT97" t="inlineStr"/>
       <c r="BU97" t="inlineStr"/>
+      <c r="BV97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -22964,6 +23203,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV98" t="n">
+        <v>1.923485570846429</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -23215,6 +23457,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV99" t="n">
+        <v>0.8977673185014454</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -23466,6 +23711,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV100" t="n">
+        <v>0.9119257803717002</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -23713,6 +23961,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV101" t="n">
+        <v>0.8558322603559853</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -23964,6 +24215,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV102" t="n">
+        <v>1.047301136525732</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -24215,6 +24469,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV103" t="n">
+        <v>1.277502508275075</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -24461,6 +24718,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV104" t="n">
+        <v>15.33110948824576</v>
       </c>
     </row>
     <row r="105">
@@ -24639,6 +24899,7 @@
       <c r="BS105" t="inlineStr"/>
       <c r="BT105" t="inlineStr"/>
       <c r="BU105" t="inlineStr"/>
+      <c r="BV105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -24886,6 +25147,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV106" t="n">
+        <v>1.058762638751214</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -25137,6 +25401,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV107" t="n">
+        <v>1.692845848941975</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -25388,6 +25655,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV108" t="n">
+        <v>1.640825792038591</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -25635,6 +25905,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV109" t="n">
+        <v>2.151559050534532</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -25885,6 +26158,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV110" t="n">
+        <v>1.044233002976706</v>
       </c>
     </row>
     <row r="111">
@@ -26063,6 +26339,7 @@
       <c r="BS111" t="inlineStr"/>
       <c r="BT111" t="inlineStr"/>
       <c r="BU111" t="inlineStr"/>
+      <c r="BV111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -26240,6 +26517,7 @@
       <c r="BS112" t="inlineStr"/>
       <c r="BT112" t="inlineStr"/>
       <c r="BU112" t="inlineStr"/>
+      <c r="BV112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -26490,6 +26768,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV113" t="n">
+        <v>1.285521573259762</v>
       </c>
     </row>
     <row r="114">
@@ -26668,6 +26949,7 @@
       <c r="BS114" t="inlineStr"/>
       <c r="BT114" t="inlineStr"/>
       <c r="BU114" t="inlineStr"/>
+      <c r="BV114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -26845,6 +27127,7 @@
       <c r="BS115" t="inlineStr"/>
       <c r="BT115" t="inlineStr"/>
       <c r="BU115" t="inlineStr"/>
+      <c r="BV115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -27026,6 +27309,7 @@
       <c r="BS116" t="inlineStr"/>
       <c r="BT116" t="inlineStr"/>
       <c r="BU116" t="inlineStr"/>
+      <c r="BV116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -27273,6 +27557,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV117" t="n">
+        <v>0.7996375571470549</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -27524,6 +27811,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV118" t="n">
+        <v>1.175799816427996</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -27771,6 +28061,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV119" t="n">
+        <v>0.6753560261939715</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -28021,6 +28314,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV120" t="n">
+        <v>1.333867912039805</v>
       </c>
     </row>
     <row r="121">
@@ -28199,6 +28495,7 @@
       <c r="BS121" t="inlineStr"/>
       <c r="BT121" t="inlineStr"/>
       <c r="BU121" t="inlineStr"/>
+      <c r="BV121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -28446,6 +28743,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV122" t="n">
+        <v>0.8831299562645438</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -28693,6 +28993,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV123" t="n">
+        <v>0.8800491952160785</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -28940,6 +29243,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV124" t="n">
+        <v>1.764836530656174</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -29191,6 +29497,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV125" t="n">
+        <v>1.180716572456894</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -29438,6 +29747,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV126" t="n">
+        <v>1.307946563398966</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -29681,6 +29993,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV127" t="n">
+        <v>1.432946296363452</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -29932,6 +30247,9 @@
           <t>Dimmer</t>
         </is>
       </c>
+      <c r="BV128" t="n">
+        <v>2.141724838407985</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -30182,6 +30500,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV129" t="n">
+        <v>0.9972522058138493</v>
       </c>
     </row>
     <row r="130">
@@ -30360,6 +30681,7 @@
       <c r="BS130" t="inlineStr"/>
       <c r="BT130" t="inlineStr"/>
       <c r="BU130" t="inlineStr"/>
+      <c r="BV130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -30537,6 +30859,7 @@
       <c r="BS131" t="inlineStr"/>
       <c r="BT131" t="inlineStr"/>
       <c r="BU131" t="inlineStr"/>
+      <c r="BV131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -30714,6 +31037,7 @@
       <c r="BS132" t="inlineStr"/>
       <c r="BT132" t="inlineStr"/>
       <c r="BU132" t="inlineStr"/>
+      <c r="BV132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -30965,6 +31289,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV133" t="n">
+        <v>0.6202382055969811</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -31212,6 +31539,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV134" t="n">
+        <v>1.511779311179392</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -31454,6 +31784,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV135" t="n">
+        <v>1.087979658581538</v>
       </c>
     </row>
     <row r="136">
@@ -31632,6 +31965,7 @@
       <c r="BS136" t="inlineStr"/>
       <c r="BT136" t="inlineStr"/>
       <c r="BU136" t="inlineStr"/>
+      <c r="BV136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -31875,6 +32209,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV137" t="n">
+        <v>1.740708543063053</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -32118,6 +32455,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV138" t="n">
+        <v>1.512048711515554</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -32369,6 +32709,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV139" t="n">
+        <v>1.311185464901675</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -32616,6 +32959,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV140" t="n">
+        <v>1.360642640965396</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -32863,6 +33209,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV141" t="n">
+        <v>1.267280025271865</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -33106,6 +33455,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV142" t="n">
+        <v>5.799355986105593</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -33353,6 +33705,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV143" t="n">
+        <v>3.98711956239338</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -33604,6 +33959,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV144" t="n">
+        <v>1.331966950745083</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -33850,6 +34208,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV145" t="n">
+        <v>1.288534896789538</v>
       </c>
     </row>
     <row r="146">
@@ -34028,6 +34389,7 @@
       <c r="BS146" t="inlineStr"/>
       <c r="BT146" t="inlineStr"/>
       <c r="BU146" t="inlineStr"/>
+      <c r="BV146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -34205,6 +34567,7 @@
       <c r="BS147" t="inlineStr"/>
       <c r="BT147" t="inlineStr"/>
       <c r="BU147" t="inlineStr"/>
+      <c r="BV147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -34448,6 +34811,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV148" t="n">
+        <v>1.525598123404499</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -34692,6 +35058,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV149" t="n">
+        <v>1.476077753040293</v>
       </c>
     </row>
     <row r="150">
@@ -34870,6 +35239,7 @@
       <c r="BS150" t="inlineStr"/>
       <c r="BT150" t="inlineStr"/>
       <c r="BU150" t="inlineStr"/>
+      <c r="BV150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -35121,6 +35491,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV151" t="n">
+        <v>1.410452435308536</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -35368,6 +35741,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV152" t="n">
+        <v>0.7646625736261637</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -35615,6 +35991,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV153" t="n">
+        <v>1.769288203916486</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -35858,6 +36237,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV154" t="n">
+        <v>1.242873675122981</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -36109,6 +36491,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV155" t="n">
+        <v>1.057853135965818</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -36355,6 +36740,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV156" t="n">
+        <v>1.698194606248821</v>
       </c>
     </row>
     <row r="157">
@@ -36537,6 +36925,7 @@
       <c r="BS157" t="inlineStr"/>
       <c r="BT157" t="inlineStr"/>
       <c r="BU157" t="inlineStr"/>
+      <c r="BV157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -36714,6 +37103,7 @@
       <c r="BS158" t="inlineStr"/>
       <c r="BT158" t="inlineStr"/>
       <c r="BU158" t="inlineStr"/>
+      <c r="BV158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -36960,6 +37350,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV159" t="n">
+        <v>1.142682681469135</v>
       </c>
     </row>
     <row r="160">
@@ -37138,6 +37531,7 @@
       <c r="BS160" t="inlineStr"/>
       <c r="BT160" t="inlineStr"/>
       <c r="BU160" t="inlineStr"/>
+      <c r="BV160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -37389,6 +37783,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV161" t="n">
+        <v>1.399704790684083</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -37640,6 +38037,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV162" t="n">
+        <v>1.128107214867612</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -37891,6 +38291,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV163" t="n">
+        <v>1.170021976973381</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -38142,6 +38545,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV164" t="n">
+        <v>1.051923153885861</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -38389,6 +38795,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV165" t="n">
+        <v>0.9830093573889346</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -38640,6 +39049,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV166" t="n">
+        <v>0.7138434285090691</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -38883,6 +39295,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV167" t="n">
+        <v>1.167970774224449</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -39126,6 +39541,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV168" t="n">
+        <v>1.284676550591598</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -39365,6 +39783,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV169" t="n">
+        <v>1.612063305269577</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -39616,6 +40037,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV170" t="n">
+        <v>1.500784955947525</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -39867,6 +40291,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV171" t="n">
+        <v>1.099376872985653</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -40117,6 +40544,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV172" t="n">
+        <v>1.088729622099013</v>
       </c>
     </row>
     <row r="173">
@@ -40295,6 +40725,7 @@
       <c r="BS173" t="inlineStr"/>
       <c r="BT173" t="inlineStr"/>
       <c r="BU173" t="inlineStr"/>
+      <c r="BV173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -40538,6 +40969,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV174" t="n">
+        <v>0.447653374698702</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -40781,6 +41215,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV175" t="n">
+        <v>0.4480441534190255</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -41028,6 +41465,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV176" t="n">
+        <v>0.6030216674512152</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -41279,6 +41719,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV177" t="n">
+        <v>0.6133974352577115</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -41526,6 +41969,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV178" t="n">
+        <v>1.370199979016798</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -41773,6 +42219,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV179" t="n">
+        <v>0.8463431046452069</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -42024,6 +42473,9 @@
           <t>Dimmer</t>
         </is>
       </c>
+      <c r="BV180" t="n">
+        <v>2.116165268735014</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -42270,6 +42722,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV181" t="n">
+        <v>0.7808249409930506</v>
       </c>
     </row>
     <row r="182">
@@ -42448,6 +42903,7 @@
       <c r="BS182" t="inlineStr"/>
       <c r="BT182" t="inlineStr"/>
       <c r="BU182" t="inlineStr"/>
+      <c r="BV182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -42625,6 +43081,7 @@
       <c r="BS183" t="inlineStr"/>
       <c r="BT183" t="inlineStr"/>
       <c r="BU183" t="inlineStr"/>
+      <c r="BV183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -42802,6 +43259,7 @@
       <c r="BS184" t="inlineStr"/>
       <c r="BT184" t="inlineStr"/>
       <c r="BU184" t="inlineStr"/>
+      <c r="BV184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -43041,6 +43499,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV185" t="n">
+        <v>0.3772490353494954</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -43284,6 +43745,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV186" t="n">
+        <v>0.6417830974195321</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -43531,6 +43995,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV187" t="n">
+        <v>1.338873202397189</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -43778,6 +44245,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV188" t="n">
+        <v>1.273472796095758</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -44029,6 +44499,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV189" t="n">
+        <v>1.424377099175682</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -44276,6 +44749,9 @@
           <t>Dimmer</t>
         </is>
       </c>
+      <c r="BV190" t="n">
+        <v>2.270157000578097</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -44527,6 +45003,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV191" t="n">
+        <v>1.558049599571859</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -44774,6 +45253,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV192" t="n">
+        <v>0.9956097406945755</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -45020,6 +45502,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV193" t="n">
+        <v>1.0487312552036</v>
       </c>
     </row>
     <row r="194">
@@ -45198,6 +45683,7 @@
       <c r="BS194" t="inlineStr"/>
       <c r="BT194" t="inlineStr"/>
       <c r="BU194" t="inlineStr"/>
+      <c r="BV194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -45449,6 +45935,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV195" t="n">
+        <v>1.558016126476089</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -45696,6 +46185,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV196" t="n">
+        <v>1.260189202720584</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -45942,6 +46434,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV197" t="n">
+        <v>1.66931607620754</v>
       </c>
     </row>
     <row r="198">
@@ -46120,6 +46615,7 @@
       <c r="BS198" t="inlineStr"/>
       <c r="BT198" t="inlineStr"/>
       <c r="BU198" t="inlineStr"/>
+      <c r="BV198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -46367,6 +46863,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV199" t="n">
+        <v>1.27188123518965</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -46613,6 +47112,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV200" t="n">
+        <v>1.697419346346643</v>
       </c>
     </row>
     <row r="201">
@@ -46791,6 +47293,7 @@
       <c r="BS201" t="inlineStr"/>
       <c r="BT201" t="inlineStr"/>
       <c r="BU201" t="inlineStr"/>
+      <c r="BV201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -46972,6 +47475,7 @@
       <c r="BS202" t="inlineStr"/>
       <c r="BT202" t="inlineStr"/>
       <c r="BU202" t="inlineStr"/>
+      <c r="BV202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -47219,6 +47723,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV203" t="n">
+        <v>1.758276581101769</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -47465,6 +47972,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV204" t="n">
+        <v>11.30379877165967</v>
       </c>
     </row>
     <row r="205">
@@ -47647,6 +48157,7 @@
       <c r="BS205" t="inlineStr"/>
       <c r="BT205" t="inlineStr"/>
       <c r="BU205" t="inlineStr"/>
+      <c r="BV205" t="inlineStr"/>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -47894,6 +48405,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV206" t="n">
+        <v>1.132142695461064</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -48145,6 +48659,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV207" t="n">
+        <v>1.304323434124897</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -48388,6 +48905,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV208" t="n">
+        <v>4.499844487953191</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -48639,6 +49159,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV209" t="n">
+        <v>0.5486073176991577</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -48890,6 +49413,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV210" t="n">
+        <v>1.718739180631414</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -49133,6 +49659,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV211" t="n">
+        <v>0.4731166715065849</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -49380,6 +49909,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV212" t="n">
+        <v>1.481980333301465</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -49631,6 +50163,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV213" t="n">
+        <v>0.6418466468345704</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -49878,6 +50413,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV214" t="n">
+        <v>1.83672036546046</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -50125,6 +50663,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV215" t="n">
+        <v>1.407060141138175</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -50376,6 +50917,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV216" t="n">
+        <v>1.152810599786382</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -50627,6 +51171,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV217" t="n">
+        <v>1.272969754500109</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -50874,6 +51421,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV218" t="n">
+        <v>9.43863530267874</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -51124,6 +51674,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV219" t="n">
+        <v>1.31532685007334</v>
       </c>
     </row>
     <row r="220">
@@ -51302,6 +51855,7 @@
       <c r="BS220" t="inlineStr"/>
       <c r="BT220" t="inlineStr"/>
       <c r="BU220" t="inlineStr"/>
+      <c r="BV220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -51548,6 +52102,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV221" t="n">
+        <v>1.36829062456463</v>
       </c>
     </row>
     <row r="222">
@@ -51726,6 +52283,7 @@
       <c r="BS222" t="inlineStr"/>
       <c r="BT222" t="inlineStr"/>
       <c r="BU222" t="inlineStr"/>
+      <c r="BV222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -51977,6 +52535,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV223" t="n">
+        <v>1.508417502543062</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -52224,6 +52785,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV224" t="n">
+        <v>2.59578443142521</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -52467,6 +53031,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV225" t="n">
+        <v>1.594044625347485</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -52714,6 +53281,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV226" t="n">
+        <v>1.112750364034412</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -52961,6 +53531,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV227" t="n">
+        <v>1.443445204341712</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -53208,6 +53781,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV228" t="n">
+        <v>1.207838360460294</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -53458,6 +54034,9 @@
         <is>
           <t>Brightest</t>
         </is>
+      </c>
+      <c r="BV229" t="n">
+        <v>0.3239496073437613</v>
       </c>
     </row>
     <row r="230">
@@ -53636,6 +54215,7 @@
       <c r="BS230" t="inlineStr"/>
       <c r="BT230" t="inlineStr"/>
       <c r="BU230" t="inlineStr"/>
+      <c r="BV230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -53813,6 +54393,7 @@
       <c r="BS231" t="inlineStr"/>
       <c r="BT231" t="inlineStr"/>
       <c r="BU231" t="inlineStr"/>
+      <c r="BV231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -54056,6 +54637,9 @@
           <t>Brightest</t>
         </is>
       </c>
+      <c r="BV232" t="n">
+        <v>1.047523443679546</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -54306,6 +54890,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV233" t="n">
+        <v>1.650395989154595</v>
       </c>
     </row>
     <row r="234">
@@ -54484,6 +55071,7 @@
       <c r="BS234" t="inlineStr"/>
       <c r="BT234" t="inlineStr"/>
       <c r="BU234" t="inlineStr"/>
+      <c r="BV234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -54734,6 +55322,9 @@
         <is>
           <t>Dim</t>
         </is>
+      </c>
+      <c r="BV235" t="n">
+        <v>1.298163184972037</v>
       </c>
     </row>
     <row r="236">
@@ -54912,6 +55503,7 @@
       <c r="BS236" t="inlineStr"/>
       <c r="BT236" t="inlineStr"/>
       <c r="BU236" t="inlineStr"/>
+      <c r="BV236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -55159,6 +55751,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV237" t="n">
+        <v>1.276640121051756</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -55410,6 +56005,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV238" t="n">
+        <v>0.7036818732168716</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -55657,6 +56255,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV239" t="n">
+        <v>0.835023861837531</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -55904,6 +56505,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV240" t="n">
+        <v>1.381414035832277</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -56150,6 +56754,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV241" t="n">
+        <v>7.249911717657366</v>
       </c>
     </row>
     <row r="242">
@@ -56328,6 +56935,7 @@
       <c r="BS242" t="inlineStr"/>
       <c r="BT242" t="inlineStr"/>
       <c r="BU242" t="inlineStr"/>
+      <c r="BV242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -56571,6 +57179,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV243" t="n">
+        <v>1.9826774960859</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -56822,6 +57433,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV244" t="n">
+        <v>1.508268843660117</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -57073,6 +57687,9 @@
           <t>Dim</t>
         </is>
       </c>
+      <c r="BV245" t="n">
+        <v>1.504793482129325</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -57324,6 +57941,9 @@
           <t>Bright</t>
         </is>
       </c>
+      <c r="BV246" t="n">
+        <v>0.9845537583908005</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -57574,6 +58194,9 @@
         <is>
           <t>Bright</t>
         </is>
+      </c>
+      <c r="BV247" t="n">
+        <v>1.28804035158083</v>
       </c>
     </row>
     <row r="248">
@@ -57752,6 +58375,7 @@
       <c r="BS248" t="inlineStr"/>
       <c r="BT248" t="inlineStr"/>
       <c r="BU248" t="inlineStr"/>
+      <c r="BV248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -57929,6 +58553,7 @@
       <c r="BS249" t="inlineStr"/>
       <c r="BT249" t="inlineStr"/>
       <c r="BU249" t="inlineStr"/>
+      <c r="BV249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -58102,6 +58727,7 @@
       <c r="BS250" t="inlineStr"/>
       <c r="BT250" t="inlineStr"/>
       <c r="BU250" t="inlineStr"/>
+      <c r="BV250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -58283,6 +58909,7 @@
       <c r="BS251" t="inlineStr"/>
       <c r="BT251" t="inlineStr"/>
       <c r="BU251" t="inlineStr"/>
+      <c r="BV251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -58460,6 +59087,7 @@
       <c r="BS252" t="inlineStr"/>
       <c r="BT252" t="inlineStr"/>
       <c r="BU252" t="inlineStr"/>
+      <c r="BV252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -58637,6 +59265,7 @@
       <c r="BS253" t="inlineStr"/>
       <c r="BT253" t="inlineStr"/>
       <c r="BU253" t="inlineStr"/>
+      <c r="BV253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -58814,6 +59443,7 @@
       <c r="BS254" t="inlineStr"/>
       <c r="BT254" t="inlineStr"/>
       <c r="BU254" t="inlineStr"/>
+      <c r="BV254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -58991,6 +59621,7 @@
       <c r="BS255" t="inlineStr"/>
       <c r="BT255" t="inlineStr"/>
       <c r="BU255" t="inlineStr"/>
+      <c r="BV255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -59172,6 +59803,7 @@
       <c r="BS256" t="inlineStr"/>
       <c r="BT256" t="inlineStr"/>
       <c r="BU256" t="inlineStr"/>
+      <c r="BV256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -59349,6 +59981,7 @@
       <c r="BS257" t="inlineStr"/>
       <c r="BT257" t="inlineStr"/>
       <c r="BU257" t="inlineStr"/>
+      <c r="BV257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -59526,6 +60159,7 @@
       <c r="BS258" t="inlineStr"/>
       <c r="BT258" t="inlineStr"/>
       <c r="BU258" t="inlineStr"/>
+      <c r="BV258" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>